<commit_message>
update 18 Junio (no dieron datos por municipio)
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>Fecha</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>2020-06-15</t>
+  </si>
+  <si>
+    <t>2020-06-16</t>
   </si>
 </sst>
 </file>
@@ -505,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,6 +1026,20 @@
         <v>14</v>
       </c>
     </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>49</v>
+      </c>
+      <c r="D37">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update 2 sept (faltan algunos datos que la junta no ha proporcionado hoy)
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="118">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -371,6 +371,12 @@
   </si>
   <si>
     <t xml:space="preserve">2020-08-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-08-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-09-01</t>
   </si>
 </sst>
 </file>
@@ -387,6 +393,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -409,6 +416,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -487,13 +495,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A81" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D111" activeCellId="0" sqref="D111"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D114" activeCellId="0" sqref="D114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.14"/>
@@ -2069,6 +2077,34 @@
         <v>69</v>
       </c>
     </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>493</v>
+      </c>
+      <c r="D113" s="0" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>522</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
update 21 oct (sin actualizacion datos IECA)
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="5">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -160,10 +160,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ205"/>
+  <dimension ref="A1:AMJ206"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D206" activeCellId="0" sqref="D206"/>
+      <selection pane="topLeft" activeCell="D207" activeCellId="0" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3379,6 +3379,20 @@
         <v>193</v>
       </c>
     </row>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="1" t="n">
+        <v>44124</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C206" s="0" t="n">
+        <v>1567</v>
+      </c>
+      <c r="D206" s="0" t="n">
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
añado datos positividad y camas ocupadas del Ministerio
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -212,18 +212,20 @@
   </sheetPr>
   <dimension ref="A1:AMJ209"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G208" activeCellId="0" sqref="G208"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G184" activeCellId="0" sqref="G184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -3145,6 +3147,18 @@
       <c r="D187" s="0" t="n">
         <v>156</v>
       </c>
+      <c r="E187" s="0" t="n">
+        <v>1158</v>
+      </c>
+      <c r="F187" s="0" t="n">
+        <v>7.05</v>
+      </c>
+      <c r="G187" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="H187" s="0" t="n">
+        <v>12.15</v>
+      </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="n">
@@ -3187,6 +3201,18 @@
       <c r="D190" s="0" t="n">
         <v>147</v>
       </c>
+      <c r="E190" s="0" t="n">
+        <v>1227</v>
+      </c>
+      <c r="F190" s="0" t="n">
+        <v>7.47</v>
+      </c>
+      <c r="G190" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="H190" s="0" t="n">
+        <v>11.33</v>
+      </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="n">
@@ -3201,6 +3227,18 @@
       <c r="D191" s="0" t="n">
         <v>149</v>
       </c>
+      <c r="E191" s="0" t="n">
+        <v>1223</v>
+      </c>
+      <c r="F191" s="0" t="n">
+        <v>7.45</v>
+      </c>
+      <c r="G191" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="H191" s="0" t="n">
+        <v>10.94</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="n">
@@ -3215,6 +3253,18 @@
       <c r="D192" s="0" t="n">
         <v>144</v>
       </c>
+      <c r="E192" s="0" t="n">
+        <v>1183</v>
+      </c>
+      <c r="F192" s="0" t="n">
+        <v>7.21</v>
+      </c>
+      <c r="G192" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="H192" s="0" t="n">
+        <v>10.81</v>
+      </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="n">
@@ -3229,6 +3279,18 @@
       <c r="D193" s="0" t="n">
         <v>139</v>
       </c>
+      <c r="E193" s="0" t="n">
+        <v>1159</v>
+      </c>
+      <c r="F193" s="0" t="n">
+        <v>7.07</v>
+      </c>
+      <c r="G193" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="H193" s="0" t="n">
+        <v>11.03</v>
+      </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="n">
@@ -3243,6 +3305,18 @@
       <c r="D194" s="0" t="n">
         <v>146</v>
       </c>
+      <c r="E194" s="0" t="n">
+        <v>1185</v>
+      </c>
+      <c r="F194" s="0" t="n">
+        <v>7.22</v>
+      </c>
+      <c r="G194" s="0" t="n">
+        <v>175</v>
+      </c>
+      <c r="H194" s="0" t="n">
+        <v>11.51</v>
+      </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="n">
@@ -3257,6 +3331,12 @@
       <c r="D195" s="0" t="n">
         <v>151</v>
       </c>
+      <c r="E195" s="0" t="n">
+        <v>1081</v>
+      </c>
+      <c r="G195" s="0" t="n">
+        <v>160</v>
+      </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="n">
@@ -3299,6 +3379,18 @@
       <c r="D198" s="0" t="n">
         <v>160</v>
       </c>
+      <c r="E198" s="0" t="n">
+        <v>1404</v>
+      </c>
+      <c r="F198" s="0" t="n">
+        <v>8.56</v>
+      </c>
+      <c r="G198" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="H198" s="0" t="n">
+        <v>12.51</v>
+      </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="n">
@@ -3313,6 +3405,18 @@
       <c r="D199" s="0" t="n">
         <v>161</v>
       </c>
+      <c r="E199" s="0" t="n">
+        <v>1409</v>
+      </c>
+      <c r="F199" s="0" t="n">
+        <v>8.59</v>
+      </c>
+      <c r="G199" s="0" t="n">
+        <v>192</v>
+      </c>
+      <c r="H199" s="0" t="n">
+        <v>12.61</v>
+      </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="n">
@@ -3327,6 +3431,18 @@
       <c r="D200" s="0" t="n">
         <v>166</v>
       </c>
+      <c r="E200" s="0" t="n">
+        <v>1449</v>
+      </c>
+      <c r="F200" s="0" t="n">
+        <v>8.82</v>
+      </c>
+      <c r="G200" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="H200" s="0" t="n">
+        <v>13.03</v>
+      </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="n">
@@ -3341,6 +3457,18 @@
       <c r="D201" s="0" t="n">
         <v>171</v>
       </c>
+      <c r="E201" s="0" t="n">
+        <v>1487</v>
+      </c>
+      <c r="F201" s="0" t="n">
+        <v>9.05</v>
+      </c>
+      <c r="G201" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="H201" s="0" t="n">
+        <v>13.79</v>
+      </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="n">
@@ -3383,6 +3511,18 @@
       <c r="D204" s="0" t="n">
         <v>188</v>
       </c>
+      <c r="E204" s="0" t="n">
+        <v>1644</v>
+      </c>
+      <c r="F204" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G204" s="0" t="n">
+        <v>219</v>
+      </c>
+      <c r="H204" s="0" t="n">
+        <v>14.32</v>
+      </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="n">
@@ -3397,6 +3537,18 @@
       <c r="D205" s="0" t="n">
         <v>193</v>
       </c>
+      <c r="E205" s="0" t="n">
+        <v>1704</v>
+      </c>
+      <c r="F205" s="0" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="G205" s="0" t="n">
+        <v>228</v>
+      </c>
+      <c r="H205" s="0" t="n">
+        <v>14.88</v>
+      </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="n">
@@ -3411,6 +3563,18 @@
       <c r="D206" s="0" t="n">
         <v>198</v>
       </c>
+      <c r="E206" s="0" t="n">
+        <v>1781</v>
+      </c>
+      <c r="F206" s="0" t="n">
+        <v>10.83</v>
+      </c>
+      <c r="G206" s="0" t="n">
+        <v>233</v>
+      </c>
+      <c r="H206" s="0" t="n">
+        <v>15.26</v>
+      </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="n">
@@ -3424,6 +3588,18 @@
       </c>
       <c r="D207" s="0" t="n">
         <v>201</v>
+      </c>
+      <c r="E207" s="0" t="n">
+        <v>1850</v>
+      </c>
+      <c r="F207" s="0" t="n">
+        <v>11.27</v>
+      </c>
+      <c r="G207" s="0" t="n">
+        <v>239</v>
+      </c>
+      <c r="H207" s="0" t="n">
+        <v>15.63</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add graficas semaforo sanidad
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -78,13 +78,13 @@
     <t xml:space="preserve">CamasOcup.Minist</t>
   </si>
   <si>
-    <t xml:space="preserve">%CamasOcup</t>
+    <t xml:space="preserve">%CamasOcup.Minist</t>
   </si>
   <si>
     <t xml:space="preserve">UCI.Minist</t>
   </si>
   <si>
-    <t xml:space="preserve">%UCI</t>
+    <t xml:space="preserve">%UCI.Minist</t>
   </si>
   <si>
     <t xml:space="preserve">Andalucía</t>
@@ -213,18 +213,18 @@
   <dimension ref="A1:AMJ209"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G184" activeCellId="0" sqref="G184"/>
+      <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="9.14"/>
   </cols>

</xml_diff>

<commit_message>
move up camas ocupada
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -212,10 +212,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ238"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H237" activeCellId="0" sqref="H237"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D238" activeCellId="0" sqref="D238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4281,6 +4281,12 @@
       <c r="B238" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="C238" s="0" t="n">
+        <v>2727</v>
+      </c>
+      <c r="D238" s="0" t="n">
+        <v>501</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update 28 dic (sin datos desde el 24)
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="9">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -210,12 +210,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ270"/>
+  <dimension ref="A1:AMJ272"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A240" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H271" activeCellId="0" sqref="H271"/>
+      <selection pane="bottomLeft" activeCell="H273" activeCellId="0" sqref="H273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5000,6 +5000,46 @@
         <v>13.84</v>
       </c>
     </row>
+    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="1" t="n">
+        <v>44190</v>
+      </c>
+      <c r="B271" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C271" s="0" t="n">
+        <v>975</v>
+      </c>
+      <c r="D271" s="0" t="n">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="1" t="n">
+        <v>44192</v>
+      </c>
+      <c r="B272" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C272" s="0" t="n">
+        <v>1016</v>
+      </c>
+      <c r="D272" s="0" t="n">
+        <v>224</v>
+      </c>
+      <c r="E272" s="0" t="n">
+        <v>1122</v>
+      </c>
+      <c r="F272" s="0" t="n">
+        <v>6.61</v>
+      </c>
+      <c r="G272" s="0" t="n">
+        <v>226</v>
+      </c>
+      <c r="H272" s="0" t="n">
+        <v>13.74</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
update 8 feb (faltan datos municipios)
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="9">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -213,9 +213,9 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H311" activeCellId="0" sqref="H311"/>
+      <selection pane="bottomLeft" activeCell="H314" activeCellId="0" sqref="H314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5900,6 +5900,32 @@
         <v>735</v>
       </c>
     </row>
+    <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="1" t="n">
+        <v>44234</v>
+      </c>
+      <c r="B313" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C313" s="0" t="n">
+        <v>4414</v>
+      </c>
+      <c r="D313" s="0" t="n">
+        <v>717</v>
+      </c>
+      <c r="E313" s="0" t="n">
+        <v>4540</v>
+      </c>
+      <c r="F313" s="0" t="n">
+        <v>25.05</v>
+      </c>
+      <c r="G313" s="0" t="n">
+        <v>719</v>
+      </c>
+      <c r="H313" s="0" t="n">
+        <v>37.23</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update 9 feb (municipios sin actualizar desde 5 feb)
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="9">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -215,7 +215,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H314" activeCellId="0" sqref="H314"/>
+      <selection pane="bottomLeft" activeCell="H315" activeCellId="0" sqref="H315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5926,6 +5926,32 @@
         <v>37.23</v>
       </c>
     </row>
+    <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="1" t="n">
+        <v>44235</v>
+      </c>
+      <c r="B314" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C314" s="0" t="n">
+        <v>4491</v>
+      </c>
+      <c r="D314" s="0" t="n">
+        <v>719</v>
+      </c>
+      <c r="E314" s="0" t="n">
+        <v>4352</v>
+      </c>
+      <c r="F314" s="0" t="n">
+        <v>24.01</v>
+      </c>
+      <c r="G314" s="0" t="n">
+        <v>717</v>
+      </c>
+      <c r="H314" s="0" t="n">
+        <v>37.11</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update 1 mar (sin datos IECA)
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="9">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -215,7 +215,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A322" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E332" activeCellId="0" sqref="E332"/>
+      <selection pane="bottomLeft" activeCell="H335" activeCellId="0" sqref="H335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6374,6 +6374,32 @@
         <v>483</v>
       </c>
     </row>
+    <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="1" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B334" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C334" s="0" t="n">
+        <v>1717</v>
+      </c>
+      <c r="D334" s="0" t="n">
+        <v>432</v>
+      </c>
+      <c r="E334" s="0" t="n">
+        <v>1802</v>
+      </c>
+      <c r="F334" s="0" t="n">
+        <v>9.96</v>
+      </c>
+      <c r="G334" s="0" t="n">
+        <v>421</v>
+      </c>
+      <c r="H334" s="0" t="n">
+        <v>21.94</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update 12 abr (faltan datos minist)
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="9">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -212,10 +212,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A361" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I373" activeCellId="0" sqref="I373"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D377" activeCellId="0" sqref="D377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7298,6 +7298,20 @@
         <v>299</v>
       </c>
     </row>
+    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="1" t="n">
+        <v>44297</v>
+      </c>
+      <c r="B376" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C376" s="0" t="n">
+        <v>1393</v>
+      </c>
+      <c r="D376" s="0" t="n">
+        <v>302</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update 12 abr (bis)
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -215,7 +215,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A361" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D377" activeCellId="0" sqref="D377"/>
+      <selection pane="bottomLeft" activeCell="E377" activeCellId="0" sqref="E377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7311,6 +7311,18 @@
       <c r="D376" s="0" t="n">
         <v>302</v>
       </c>
+      <c r="E376" s="0" t="n">
+        <v>1508</v>
+      </c>
+      <c r="F376" s="0" t="n">
+        <v>8.32</v>
+      </c>
+      <c r="G376" s="0" t="n">
+        <v>293</v>
+      </c>
+      <c r="H376" s="0" t="n">
+        <v>15.45</v>
+      </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
update 13 abr (sin IECA)
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="9">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -215,7 +215,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A361" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E377" activeCellId="0" sqref="E377"/>
+      <selection pane="bottomLeft" activeCell="H378" activeCellId="0" sqref="H378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7324,6 +7324,32 @@
         <v>15.45</v>
       </c>
     </row>
+    <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A377" s="1" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B377" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C377" s="0" t="n">
+        <v>1473</v>
+      </c>
+      <c r="D377" s="0" t="n">
+        <v>297</v>
+      </c>
+      <c r="E377" s="0" t="n">
+        <v>1496</v>
+      </c>
+      <c r="F377" s="0" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="G377" s="0" t="n">
+        <v>286</v>
+      </c>
+      <c r="H377" s="0" t="n">
+        <v>15.08</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update 5 jul bis
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -213,9 +213,9 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A446" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A449" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H458" activeCellId="0" sqref="H458"/>
+      <selection pane="bottomLeft" activeCell="C461" activeCellId="0" sqref="C461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9201,6 +9201,24 @@
       <c r="B460" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="C460" s="0" t="n">
+        <v>487</v>
+      </c>
+      <c r="D460" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="E460" s="0" t="n">
+        <v>530</v>
+      </c>
+      <c r="F460" s="0" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="G460" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="H460" s="0" t="n">
+        <v>6.48</v>
+      </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
update 28 jul (falta datos Minist)
</commit_message>
<xml_diff>
--- a/datos/camas_ocupadas.xlsx
+++ b/datos/camas_ocupadas.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="9">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -215,7 +215,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A468" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H480" activeCellId="0" sqref="H480"/>
+      <selection pane="bottomLeft" activeCell="E480" activeCellId="0" sqref="E480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9678,6 +9678,20 @@
         <v>10.96</v>
       </c>
     </row>
+    <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="1" t="n">
+        <v>44404</v>
+      </c>
+      <c r="B480" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C480" s="0" t="n">
+        <v>1151</v>
+      </c>
+      <c r="D480" s="0" t="n">
+        <v>197</v>
+      </c>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>